<commit_message>
Latest selenium version added, removed webdriver manager
</commit_message>
<xml_diff>
--- a/RunData/testData.xlsx
+++ b/RunData/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\booba\git\Weather_Project\RunData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\booba\IdeaProjects\Weather_Project\RunData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F948AD5A-F025-4BF7-9798-1F638309388D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA442B75-4151-4C31-A746-EF1D1134E6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RunSheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>City</t>
   </si>
@@ -74,12 +74,6 @@
   </si>
   <si>
     <t>Browser</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Firefox</t>
   </si>
   <si>
     <t>Edge</t>
@@ -145,13 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,162 +422,162 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>20</v>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3" t="s">

</xml_diff>